<commit_message>
De-anonymize and add README
</commit_message>
<xml_diff>
--- a/raw_results/raw_results_app2_model-supported.xlsx
+++ b/raw_results/raw_results_app2_model-supported.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simon/Documents/Own/Papers_and_Projects/empirical_study_DFDs/GitHub_replication_package/raw_results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{626EDB9A-4443-0B43-9F9B-C7BE1F443FB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF0E4E2A-517E-7641-AB49-8C2BB062909E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Formularantworten 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="145">
   <si>
     <t>Zeitstempel</t>
   </si>
@@ -228,9 +228,6 @@
   </si>
   <si>
     <t>It is easier to find the general information and to know where to search in the code if more details are needed. But it lacks maybe a bit of details that confuse when comparing with the code. I think it's an overall useful tool to have, but I wouldn't rely solely on it.</t>
-  </si>
-  <si>
-    <t>Paula Köppe</t>
   </si>
   <si>
     <t>Traceability Information, Documentation</t>
@@ -544,7 +541,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -552,8 +549,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -774,9 +770,9 @@
   </sheetPr>
   <dimension ref="A1:AC12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AE1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Z13" sqref="Z13"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -878,7 +874,7 @@
         <v>44944.425130451389</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>18</v>
@@ -886,8 +882,8 @@
       <c r="D2" s="1">
         <v>8765</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>107</v>
+      <c r="E2" t="s">
+        <v>106</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>19</v>
@@ -895,8 +891,8 @@
       <c r="G2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="5" t="s">
-        <v>108</v>
+      <c r="H2" t="s">
+        <v>107</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>21</v>
@@ -907,8 +903,8 @@
       <c r="K2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="5" t="s">
-        <v>109</v>
+      <c r="L2" t="s">
+        <v>108</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>24</v>
@@ -917,7 +913,7 @@
         <v>25</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>26</v>
@@ -929,7 +925,7 @@
         <v>27</v>
       </c>
       <c r="S2" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="T2" s="1" t="s">
         <v>24</v>
@@ -941,7 +937,7 @@
         <v>22</v>
       </c>
       <c r="W2" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="X2" s="1" t="s">
         <v>26</v>
@@ -949,8 +945,8 @@
       <c r="Y2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="Z2" s="5" t="s">
-        <v>113</v>
+      <c r="Z2" t="s">
+        <v>112</v>
       </c>
       <c r="AA2" s="1" t="s">
         <v>24</v>
@@ -967,7 +963,7 @@
         <v>44944.431504594904</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>32</v>
@@ -976,7 +972,7 @@
         <v>33306</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>21</v>
@@ -985,7 +981,7 @@
         <v>33</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>34</v>
@@ -997,7 +993,7 @@
         <v>22</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>34</v>
@@ -1006,7 +1002,7 @@
         <v>35</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>36</v>
@@ -1018,7 +1014,7 @@
         <v>27</v>
       </c>
       <c r="S3" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="T3" s="1" t="s">
         <v>21</v>
@@ -1030,7 +1026,7 @@
         <v>22</v>
       </c>
       <c r="W3" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="X3" s="1" t="s">
         <v>34</v>
@@ -1039,7 +1035,7 @@
         <v>37</v>
       </c>
       <c r="Z3" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AA3" s="1" t="s">
         <v>34</v>
@@ -1056,7 +1052,7 @@
         <v>44944.433311377317</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>40</v>
@@ -1064,8 +1060,8 @@
       <c r="D4" s="1">
         <v>8765</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>118</v>
+      <c r="E4" t="s">
+        <v>117</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>36</v>
@@ -1073,8 +1069,8 @@
       <c r="G4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="H4" s="5" t="s">
-        <v>119</v>
+      <c r="H4" t="s">
+        <v>118</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>42</v>
@@ -1085,8 +1081,8 @@
       <c r="K4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="L4" s="5" t="s">
-        <v>120</v>
+      <c r="L4" t="s">
+        <v>119</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>36</v>
@@ -1095,7 +1091,7 @@
         <v>43</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="P4" s="1" t="s">
         <v>24</v>
@@ -1107,7 +1103,7 @@
         <v>27</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="T4" s="1" t="s">
         <v>45</v>
@@ -1119,7 +1115,7 @@
         <v>22</v>
       </c>
       <c r="W4" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="X4" s="1" t="s">
         <v>46</v>
@@ -1127,8 +1123,8 @@
       <c r="Y4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="Z4" s="5" t="s">
-        <v>124</v>
+      <c r="Z4" t="s">
+        <v>123</v>
       </c>
       <c r="AA4" s="1" t="s">
         <v>21</v>
@@ -1145,7 +1141,7 @@
         <v>44944.433484884255</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>40</v>
@@ -1153,8 +1149,8 @@
       <c r="D5" s="1">
         <v>8765</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>118</v>
+      <c r="E5" t="s">
+        <v>117</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>21</v>
@@ -1162,8 +1158,8 @@
       <c r="G5" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="H5" s="5" t="s">
-        <v>125</v>
+      <c r="H5" t="s">
+        <v>124</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>21</v>
@@ -1175,7 +1171,7 @@
         <v>27</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>21</v>
@@ -1184,7 +1180,7 @@
         <v>51</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="P5" s="1" t="s">
         <v>36</v>
@@ -1196,7 +1192,7 @@
         <v>27</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="T5" s="1" t="s">
         <v>21</v>
@@ -1208,7 +1204,7 @@
         <v>22</v>
       </c>
       <c r="W5" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="X5" s="1" t="s">
         <v>21</v>
@@ -1217,7 +1213,7 @@
         <v>52</v>
       </c>
       <c r="Z5" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AA5" s="1" t="s">
         <v>21</v>
@@ -1234,7 +1230,7 @@
         <v>44944.434452881949</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>54</v>
@@ -1242,8 +1238,8 @@
       <c r="D6" s="1">
         <v>8765</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>97</v>
+      <c r="E6" t="s">
+        <v>96</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>30</v>
@@ -1251,8 +1247,8 @@
       <c r="G6" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="H6" s="6" t="s">
-        <v>104</v>
+      <c r="H6" s="5" t="s">
+        <v>103</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>34</v>
@@ -1263,8 +1259,8 @@
       <c r="K6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="L6" s="6" t="s">
-        <v>104</v>
+      <c r="L6" s="5" t="s">
+        <v>103</v>
       </c>
       <c r="M6" s="1" t="s">
         <v>34</v>
@@ -1272,8 +1268,8 @@
       <c r="N6" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="O6" s="6" t="s">
-        <v>144</v>
+      <c r="O6" s="5" t="s">
+        <v>143</v>
       </c>
       <c r="P6" s="1" t="s">
         <v>30</v>
@@ -1284,8 +1280,8 @@
       <c r="R6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="S6" s="6" t="s">
-        <v>144</v>
+      <c r="S6" s="5" t="s">
+        <v>143</v>
       </c>
       <c r="T6" s="1" t="s">
         <v>30</v>
@@ -1296,8 +1292,8 @@
       <c r="V6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="W6" s="6" t="s">
-        <v>104</v>
+      <c r="W6" s="5" t="s">
+        <v>103</v>
       </c>
       <c r="X6" s="1" t="s">
         <v>34</v>
@@ -1305,8 +1301,8 @@
       <c r="Y6" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="Z6" s="6" t="s">
-        <v>144</v>
+      <c r="Z6" s="5" t="s">
+        <v>143</v>
       </c>
       <c r="AA6" s="1" t="s">
         <v>30</v>
@@ -1323,7 +1319,7 @@
         <v>44944.437197372681</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>60</v>
@@ -1331,8 +1327,8 @@
       <c r="D7" s="1">
         <v>8765</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>107</v>
+      <c r="E7" t="s">
+        <v>106</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>19</v>
@@ -1340,8 +1336,8 @@
       <c r="G7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H7" s="5" t="s">
-        <v>130</v>
+      <c r="H7" t="s">
+        <v>129</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>61</v>
@@ -1353,7 +1349,7 @@
         <v>27</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M7" s="1" t="s">
         <v>26</v>
@@ -1373,8 +1369,8 @@
       <c r="R7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="S7" s="5" t="s">
-        <v>98</v>
+      <c r="S7" t="s">
+        <v>97</v>
       </c>
       <c r="T7" s="1" t="s">
         <v>30</v>
@@ -1386,7 +1382,7 @@
         <v>22</v>
       </c>
       <c r="W7" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="X7" s="1" t="s">
         <v>24</v>
@@ -1394,8 +1390,8 @@
       <c r="Y7" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="Z7" s="6" t="s">
-        <v>145</v>
+      <c r="Z7" s="5" t="s">
+        <v>144</v>
       </c>
       <c r="AA7" s="1" t="s">
         <v>65</v>
@@ -1412,16 +1408,14 @@
         <v>44944.45268869213</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>68</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="C8" s="1"/>
       <c r="D8" s="1">
         <v>8765</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>19</v>
@@ -1430,10 +1424,10 @@
         <v>33</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>22</v>
@@ -1442,16 +1436,16 @@
         <v>27</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M8" s="1" t="s">
         <v>26</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="P8" s="1" t="s">
         <v>26</v>
@@ -1462,8 +1456,8 @@
       <c r="R8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="S8" s="5" t="s">
-        <v>134</v>
+      <c r="S8" t="s">
+        <v>133</v>
       </c>
       <c r="T8" s="1" t="s">
         <v>45</v>
@@ -1475,22 +1469,22 @@
         <v>22</v>
       </c>
       <c r="W8" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="X8" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="Y8" s="1" t="s">
         <v>37</v>
       </c>
       <c r="Z8" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AA8" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AB8" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="AB8" s="3" t="s">
-        <v>72</v>
       </c>
       <c r="AC8" s="1" t="s">
         <v>48</v>
@@ -1501,16 +1495,16 @@
         <v>44945.495154456017</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D9" s="1">
         <v>8765</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>30</v>
@@ -1519,28 +1513,28 @@
         <v>33</v>
       </c>
       <c r="H9" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L9" t="s">
         <v>103</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L9" s="5" t="s">
-        <v>104</v>
       </c>
       <c r="M9" s="1" t="s">
         <v>34</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="O9" s="5" t="s">
-        <v>97</v>
+        <v>73</v>
+      </c>
+      <c r="O9" t="s">
+        <v>96</v>
       </c>
       <c r="P9" s="1" t="s">
         <v>30</v>
@@ -1551,8 +1545,8 @@
       <c r="R9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="S9" s="5" t="s">
-        <v>97</v>
+      <c r="S9" t="s">
+        <v>96</v>
       </c>
       <c r="T9" s="1" t="s">
         <v>30</v>
@@ -1564,25 +1558,25 @@
         <v>22</v>
       </c>
       <c r="W9" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="X9" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="Y9" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="Z9" s="5" t="s">
-        <v>104</v>
+      <c r="Z9" t="s">
+        <v>103</v>
       </c>
       <c r="AA9" s="1" t="s">
         <v>34</v>
       </c>
       <c r="AB9" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AC9" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="AC9" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1590,25 +1584,25 @@
         <v>44945.498403784717</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D10" s="1">
         <v>8765</v>
       </c>
-      <c r="E10" s="5" t="s">
-        <v>97</v>
+      <c r="E10" t="s">
+        <v>96</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>30</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>136</v>
+        <v>77</v>
+      </c>
+      <c r="H10" t="s">
+        <v>135</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>21</v>
@@ -1619,59 +1613,59 @@
       <c r="K10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="L10" s="5" t="s">
-        <v>97</v>
+      <c r="L10" t="s">
+        <v>96</v>
       </c>
       <c r="M10" s="1" t="s">
         <v>30</v>
       </c>
       <c r="N10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="O10" t="s">
+        <v>96</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S10" t="s">
+        <v>96</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="U10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="V10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="W10" t="s">
+        <v>96</v>
+      </c>
+      <c r="X10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y10" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="O10" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="R10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="S10" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="T10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="U10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="V10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="W10" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="X10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="Y10" s="1" t="s">
+      <c r="Z10" t="s">
+        <v>96</v>
+      </c>
+      <c r="AA10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB10" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="Z10" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="AA10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AB10" s="3" t="s">
+      <c r="AC10" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="AC10" s="1" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1679,25 +1673,25 @@
         <v>44945.512097453699</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D11" s="1">
         <v>8765</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>19</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>21</v>
@@ -1708,17 +1702,17 @@
       <c r="K11" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="L11" s="5" t="s">
-        <v>97</v>
+      <c r="L11" t="s">
+        <v>96</v>
       </c>
       <c r="M11" s="1" t="s">
         <v>30</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="O11" s="5" t="s">
-        <v>97</v>
+        <v>84</v>
+      </c>
+      <c r="O11" t="s">
+        <v>96</v>
       </c>
       <c r="P11" s="1" t="s">
         <v>30</v>
@@ -1730,7 +1724,7 @@
         <v>27</v>
       </c>
       <c r="S11" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="T11" s="1" t="s">
         <v>30</v>
@@ -1741,8 +1735,8 @@
       <c r="V11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="W11" s="5" t="s">
-        <v>97</v>
+      <c r="W11" t="s">
+        <v>96</v>
       </c>
       <c r="X11" s="1" t="s">
         <v>30</v>
@@ -1750,17 +1744,17 @@
       <c r="Y11" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="Z11" s="5" t="s">
-        <v>97</v>
+      <c r="Z11" t="s">
+        <v>96</v>
       </c>
       <c r="AA11" s="1" t="s">
         <v>30</v>
       </c>
       <c r="AB11" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC11" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="AC11" s="1" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1768,16 +1762,16 @@
         <v>44945.518396608793</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D12" s="1">
         <v>8765</v>
       </c>
-      <c r="E12" s="5" t="s">
-        <v>107</v>
+      <c r="E12" t="s">
+        <v>106</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>19</v>
@@ -1785,11 +1779,11 @@
       <c r="G12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H12" s="5" t="s">
-        <v>130</v>
+      <c r="H12" t="s">
+        <v>129</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>22</v>
@@ -1797,17 +1791,17 @@
       <c r="K12" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="L12" s="5" t="s">
-        <v>139</v>
+      <c r="L12" t="s">
+        <v>138</v>
       </c>
       <c r="M12" s="1" t="s">
         <v>26</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="O12" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="P12" s="1" t="s">
         <v>26</v>
@@ -1819,7 +1813,7 @@
         <v>27</v>
       </c>
       <c r="S12" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="T12" s="1" t="s">
         <v>26</v>
@@ -1831,7 +1825,7 @@
         <v>22</v>
       </c>
       <c r="W12" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="X12" s="1" t="s">
         <v>26</v>
@@ -1839,17 +1833,17 @@
       <c r="Y12" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="Z12" s="5" t="s">
-        <v>124</v>
+      <c r="Z12" t="s">
+        <v>123</v>
       </c>
       <c r="AA12" s="1" t="s">
         <v>65</v>
       </c>
       <c r="AB12" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="AC12" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="AC12" s="1" t="s">
-        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>